<commit_message>
+ Fixed issue on U2 and U5, added battery to the schematic and BOM
</commit_message>
<xml_diff>
--- a/hydSmart_VA/Release/VC/03_BOM/Bill of Materials-Hydrosmart Revised Schematics_2025-05-28T19_57_34_UTC.xlsx
+++ b/hydSmart_VA/Release/VC/03_BOM/Bill of Materials-Hydrosmart Revised Schematics_2025-05-28T19_57_34_UTC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2025\Altium\LuHan\Hydrosmart\2025-07-02\Project Outputs\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2025\Altium\LuHan\Hydrosmart\2025-07-14\hydSmart_VA\Release\VC\03_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1944E5A-1110-402A-958E-32D3DE3441EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF43D44-D37F-4645-8C04-C66EF7CEAE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
   <si>
     <t>Approved</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Designator</t>
   </si>
   <si>
+    <t>BT1</t>
+  </si>
+  <si>
     <t>C1</t>
   </si>
   <si>
@@ -64,15 +67,24 @@
     <t>U1</t>
   </si>
   <si>
+    <t>U2</t>
+  </si>
+  <si>
     <t>U3, U4</t>
   </si>
   <si>
+    <t>U5</t>
+  </si>
+  <si>
     <t>Y1</t>
   </si>
   <si>
     <t>Comment</t>
   </si>
   <si>
+    <t>Battery</t>
+  </si>
+  <si>
     <t>47uF</t>
   </si>
   <si>
@@ -106,12 +118,18 @@
     <t>CT8122AM-IS3</t>
   </si>
   <si>
+    <t>112TR</t>
+  </si>
+  <si>
     <t>FC-135_32.7680KA-AG5</t>
   </si>
   <si>
     <t>Footprint</t>
   </si>
   <si>
+    <t>BAT-2</t>
+  </si>
+  <si>
     <t>FP-C2012-125-0_2-MFG</t>
   </si>
   <si>
@@ -142,6 +160,9 @@
     <t>Description</t>
   </si>
   <si>
+    <t>BATTERY LITHIUM 3V COIN 24.5MM</t>
+  </si>
+  <si>
     <t>Multilayer Ceramic Capacitors 47μF ±20% 6.3V X5R SMD 0805</t>
   </si>
   <si>
@@ -169,15 +190,24 @@
     <t>Integrated Circuit</t>
   </si>
   <si>
+    <t>BATT CONTACT SOLID MULTIPLE SMD</t>
+  </si>
+  <si>
     <t>Integrated Bipolar TMR Digital Latch</t>
   </si>
   <si>
+    <t>BATT CONTACT SPRING MULTIPLE SMD</t>
+  </si>
+  <si>
     <t>Crystal or Oscillator</t>
   </si>
   <si>
     <t>Manufacturer_Name</t>
   </si>
   <si>
+    <t>Jauch Quartz</t>
+  </si>
+  <si>
     <t>Taiyo Yuden</t>
   </si>
   <si>
@@ -199,6 +229,9 @@
     <t>Analog Devices</t>
   </si>
   <si>
+    <t>Keystone Electronics</t>
+  </si>
+  <si>
     <t>Allegro MicroSystems</t>
   </si>
   <si>
@@ -206,6 +239,9 @@
   </si>
   <si>
     <t>Manufacturer_Part_Number</t>
+  </si>
+  <si>
+    <t>CR2477</t>
   </si>
   <si>
     <t>JMK212BBJ476MG-T</t>
@@ -402,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -429,13 +465,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -447,9 +477,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -475,6 +502,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,8 +640,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:G16" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:G16" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:G19" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:G19" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Quantity"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Designator"/>
@@ -915,7 +945,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -925,341 +955,410 @@
   <cols>
     <col min="1" max="1" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="78.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>60</v>
+      <c r="C1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>16</v>
+      <c r="C2" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="20">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15">
+      <c r="G3" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20">
         <v>1</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15">
-        <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>18</v>
+      <c r="C4" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="15">
-        <v>1</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="20">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>19</v>
+      <c r="C5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15">
+      <c r="A6" s="20">
         <v>1</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>20</v>
+      <c r="C6" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+        <v>49</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15">
+      <c r="A7" s="20">
         <v>1</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>64</v>
-      </c>
+      <c r="C7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15">
+      <c r="A8" s="20">
         <v>1</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>22</v>
+      <c r="C8" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="15">
+      <c r="A9" s="20">
         <v>1</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="11" t="s">
+      <c r="C9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>65</v>
       </c>
+      <c r="G9" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15">
-        <v>2</v>
+      <c r="A10" s="20">
+        <v>1</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>24</v>
+      <c r="C10" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="G10" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="20">
+        <v>2</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15">
+      <c r="G11" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="20">
         <v>1</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15">
-        <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>26</v>
+      <c r="C12" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="F12" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="20">
+        <v>1</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="9">
+        <v>122</v>
+      </c>
+      <c r="D13" s="9">
+        <v>122</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="9">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="20">
+        <v>2</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="20">
+        <v>1</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="20">
+        <v>1</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="15">
-        <v>1</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" customFormat="1" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="22">
-        <f>SUM(A2:A13)</f>
-        <v>15</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="1:7" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+      <c r="F16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" customFormat="1" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19">
+        <f>SUM(A2:A16)</f>
+        <v>18</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>